<commit_message>
Added the ER-diagram and and a excel spreadsheet with tables for attributes
</commit_message>
<xml_diff>
--- a/planningDocs/Rational Schema.xlsx
+++ b/planningDocs/Rational Schema.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28300" windowHeight="12080" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="0.9" sheetId="2" r:id="rId1"/>
+    <sheet name="v0.5" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Employee</t>
   </si>
@@ -175,13 +176,106 @@
   </si>
   <si>
     <t>Holidays_taken</t>
+  </si>
+  <si>
+    <t>Msg_from_E-ID</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>H-ID</t>
+  </si>
+  <si>
+    <t>D-Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Repeats</t>
+  </si>
+  <si>
+    <t>Hoplidays_held</t>
+  </si>
+  <si>
+    <t>Pay_Type</t>
+  </si>
+  <si>
+    <t>Pay_Type-ID</t>
+  </si>
+  <si>
+    <t>Pay_type_when over time</t>
+  </si>
+  <si>
+    <t>Pay_Type in Departments</t>
+  </si>
+  <si>
+    <t>Punch</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Mesagge</t>
+  </si>
+  <si>
+    <t>P-ID</t>
+  </si>
+  <si>
+    <t>In-time</t>
+  </si>
+  <si>
+    <t>out-time</t>
+  </si>
+  <si>
+    <t>Punch_type-ID</t>
+  </si>
+  <si>
+    <t>Timecard</t>
+  </si>
+  <si>
+    <t>Timecard Lines</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Split-Start</t>
+  </si>
+  <si>
+    <t>Split-End</t>
+  </si>
+  <si>
+    <t>Punch_Type</t>
+  </si>
+  <si>
+    <t>Punch_Type-ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>punch_in_option</t>
+  </si>
+  <si>
+    <t>Line-Number</t>
+  </si>
+  <si>
+    <t>More?</t>
+  </si>
+  <si>
+    <t>Not totally sure how to make this in a good way</t>
+  </si>
+  <si>
+    <t>Derpartment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -213,6 +307,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +332,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -239,22 +340,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -584,10 +713,381 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>60</v>
+      </c>
+      <c r="G56" t="s">
+        <v>73</v>
+      </c>
+      <c r="H56" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B50:H50"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -604,15 +1104,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="2:8">
       <c r="B3" s="1" t="s">
@@ -638,15 +1138,15 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="1" t="s">
@@ -672,18 +1172,18 @@
       </c>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="3"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="1" t="s">
@@ -709,15 +1209,15 @@
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="1" t="s">
@@ -734,15 +1234,15 @@
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="1" t="s">
@@ -759,18 +1259,18 @@
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -784,15 +1284,15 @@
       </c>
     </row>
     <row r="26" spans="2:8">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="2:8">
       <c r="B27" s="1" t="s">
@@ -803,15 +1303,15 @@
       </c>
     </row>
     <row r="30" spans="2:8">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="1" t="s">
@@ -825,15 +1325,15 @@
       </c>
     </row>
     <row r="34" spans="2:8">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="1" t="s">
@@ -844,15 +1344,15 @@
       </c>
     </row>
     <row r="38" spans="2:8">
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="1" t="s">
@@ -869,15 +1369,15 @@
       </c>
     </row>
     <row r="42" spans="2:8">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="1" t="s">
@@ -891,15 +1391,15 @@
       </c>
     </row>
     <row r="46" spans="2:8">
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="1" t="s">
@@ -911,18 +1411,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B14:H14"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B26:H26"/>
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B46:H46"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added the import of the ER-diagram, and underlined primary keys in the Rational Schema.
</commit_message>
<xml_diff>
--- a/planningDocs/Rational Schema.xlsx
+++ b/planningDocs/Rational Schema.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28305" windowHeight="12075" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="0.9" sheetId="2" r:id="rId1"/>
@@ -314,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,6 +353,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -368,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -378,29 +385,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -409,12 +416,21 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -432,8 +448,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -441,22 +471,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -465,6 +502,13 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -473,6 +517,13 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -810,358 +861,351 @@
   <dimension ref="B2:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B7" sqref="B7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
-    <col min="4" max="4" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="16.125" customWidth="1"/>
-    <col min="9" max="9" width="15.375" customWidth="1"/>
+    <col min="2" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:9">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="2:9">
       <c r="B3" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="E3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="2:9">
+      <c r="B7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:9">
+      <c r="B11" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="2:9">
+      <c r="B16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="2:8">
+      <c r="B21" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+    <row r="30" spans="2:8">
+      <c r="B30" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="11"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="10"/>
+    </row>
+    <row r="34" spans="2:8">
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+    <row r="35" spans="2:8">
+      <c r="B35" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
+      <c r="C35" s="9"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
+    <row r="40" spans="2:8">
+      <c r="B40" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+    <row r="45" spans="2:8">
+      <c r="B45" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="11"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="2:8">
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8">
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
+    <row r="50" spans="2:8">
+      <c r="B50" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+      <c r="C50" s="9"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
+    <row r="55" spans="2:8">
+      <c r="B55" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="G56" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="H56" s="7" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="D8:E8"/>
+  <mergeCells count="16">
+    <mergeCell ref="E22:G22"/>
     <mergeCell ref="B55:H55"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="E31:F31"/>
@@ -1171,6 +1215,12 @@
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1190,31 +1240,31 @@
       <selection activeCell="B26" sqref="B26:H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="1"/>
-    <col min="2" max="2" width="13.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.875" style="1"/>
+    <col min="7" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:8">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="2:8">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1237,18 +1287,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="2:8">
+      <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1271,21 +1321,21 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="2:8">
+      <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="2:8">
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1308,18 +1358,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+    <row r="14" spans="2:8">
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="2:8">
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1333,18 +1383,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="2:8">
+      <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:8">
       <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
@@ -1358,18 +1408,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:8">
+      <c r="B22" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="2:8">
       <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1383,18 +1433,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+    <row r="26" spans="2:8">
+      <c r="B26" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" spans="2:8">
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1402,18 +1452,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="2:8">
+      <c r="B30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="2:8">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
@@ -1424,18 +1474,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+    <row r="34" spans="2:8">
+      <c r="B34" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+    </row>
+    <row r="35" spans="2:8">
       <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1443,18 +1493,18 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="2:8">
+      <c r="B38" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="2:8">
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1468,18 +1518,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
+    <row r="42" spans="2:8">
+      <c r="B42" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="2:8">
       <c r="B43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1490,18 +1540,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
+    <row r="46" spans="2:8">
+      <c r="B46" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+    </row>
+    <row r="47" spans="2:8">
       <c r="B47" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
changes to relational schema
</commit_message>
<xml_diff>
--- a/planningDocs/Rational Schema.xlsx
+++ b/planningDocs/Rational Schema.xlsx
@@ -314,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -349,6 +349,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -433,7 +441,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -442,19 +450,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -810,7 +820,7 @@
   <dimension ref="B2:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -826,40 +836,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -873,21 +883,21 @@
       <c r="H4" s="1"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -899,71 +909,71 @@
       <c r="H8" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>80</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -971,43 +981,43 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="8" t="s">
         <v>83</v>
       </c>
       <c r="E31" s="11" t="s">
@@ -1019,70 +1029,70 @@
       <c r="B34" s="4"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="9"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="7"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="8" t="s">
         <v>89</v>
       </c>
       <c r="D46" s="11" t="s">
@@ -1099,69 +1109,63 @@
       <c r="E48" s="3"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E56" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G56" s="10" t="s">
+      <c r="G56" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="H56" s="8" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="D8:E8"/>
     <mergeCell ref="B55:H55"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="E31:F31"/>
@@ -1171,9 +1175,15 @@
     <mergeCell ref="B40:G40"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1204,15 +1214,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1238,15 +1248,15 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1275,15 +1285,15 @@
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -1309,15 +1319,15 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -1334,15 +1344,15 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -1359,15 +1369,15 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
@@ -1384,15 +1394,15 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
@@ -1403,15 +1413,15 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -1425,15 +1435,15 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
@@ -1444,15 +1454,15 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
@@ -1469,15 +1479,15 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
@@ -1491,15 +1501,15 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">

</xml_diff>